<commit_message>
add results and plots
</commit_message>
<xml_diff>
--- a/data_output/HBSC_DNSSSU/MPALC/insp_desc_20210817_None_[8, 40, 3, 20]_[0.05, 1.0]_[True, 10]_[0.9, 80]_['prev', 'data', None, None, 'max', None, 'max', 1].xlsx
+++ b/data_output/HBSC_DNSSSU/MPALC/insp_desc_20210817_None_[8, 40, 3, 20]_[0.05, 1.0]_[True, 10]_[0.9, 80]_['prev', 'data', None, None, 'max', None, 'max', 1].xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="sgs" sheetId="1" r:id="rId1"/>
     <sheet name="jsmatrix" sheetId="2" r:id="rId2"/>
+    <sheet name="params" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="87">
   <si>
     <t>sg</t>
   </si>
@@ -111,6 +112,171 @@
   </si>
   <si>
     <t>{'lft': (15.0, 16.0), 'etngroep3': (0.0, ' Westers')}</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>prev</t>
+  </si>
+  <si>
+    <t>prev_se</t>
+  </si>
+  <si>
+    <t>min_size</t>
+  </si>
+  <si>
+    <t>condition11</t>
+  </si>
+  <si>
+    <t>condition12</t>
+  </si>
+  <si>
+    <t>condition13</t>
+  </si>
+  <si>
+    <t>condition21</t>
+  </si>
+  <si>
+    <t>condition22</t>
+  </si>
+  <si>
+    <t>condition23</t>
+  </si>
+  <si>
+    <t>condition31</t>
+  </si>
+  <si>
+    <t>condition32</t>
+  </si>
+  <si>
+    <t>condition33</t>
+  </si>
+  <si>
+    <t>condition41</t>
+  </si>
+  <si>
+    <t>condition42</t>
+  </si>
+  <si>
+    <t>condition43</t>
+  </si>
+  <si>
+    <t>condition51</t>
+  </si>
+  <si>
+    <t>condition52</t>
+  </si>
+  <si>
+    <t>condition53</t>
+  </si>
+  <si>
+    <t>condition61</t>
+  </si>
+  <si>
+    <t>condition62</t>
+  </si>
+  <si>
+    <t>condition63</t>
+  </si>
+  <si>
+    <t>condition71</t>
+  </si>
+  <si>
+    <t>condition72</t>
+  </si>
+  <si>
+    <t>condition81</t>
+  </si>
+  <si>
+    <t>condition82</t>
+  </si>
+  <si>
+    <t>condition83</t>
+  </si>
+  <si>
+    <t>condition91</t>
+  </si>
+  <si>
+    <t>condition92</t>
+  </si>
+  <si>
+    <t>condition101</t>
+  </si>
+  <si>
+    <t>condition102</t>
+  </si>
+  <si>
+    <t>condition103</t>
+  </si>
+  <si>
+    <t>condition111</t>
+  </si>
+  <si>
+    <t>condition112</t>
+  </si>
+  <si>
+    <t>condition113</t>
+  </si>
+  <si>
+    <t>condition121</t>
+  </si>
+  <si>
+    <t>condition122</t>
+  </si>
+  <si>
+    <t>condition131</t>
+  </si>
+  <si>
+    <t>condition132</t>
+  </si>
+  <si>
+    <t>condition133</t>
+  </si>
+  <si>
+    <t>condition141</t>
+  </si>
+  <si>
+    <t>condition151</t>
+  </si>
+  <si>
+    <t>condition152</t>
+  </si>
+  <si>
+    <t>condition161</t>
+  </si>
+  <si>
+    <t>condition162</t>
+  </si>
+  <si>
+    <t>condition171</t>
+  </si>
+  <si>
+    <t>condition172</t>
+  </si>
+  <si>
+    <t>condition173</t>
+  </si>
+  <si>
+    <t>condition181</t>
+  </si>
+  <si>
+    <t>condition182</t>
+  </si>
+  <si>
+    <t>condition191</t>
+  </si>
+  <si>
+    <t>condition192</t>
+  </si>
+  <si>
+    <t>condition201</t>
+  </si>
+  <si>
+    <t>condition202</t>
+  </si>
+  <si>
+    <t>meting</t>
   </si>
 </sst>
 </file>
@@ -2962,4 +3128,1687 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:BC10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:55">
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55">
+      <c r="A2" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B2">
+        <v>4402</v>
+      </c>
+      <c r="C2">
+        <v>0.5533848250795094</v>
+      </c>
+      <c r="D2">
+        <v>0.007493844485279851</v>
+      </c>
+      <c r="E2">
+        <v>220.1</v>
+      </c>
+      <c r="F2">
+        <v>0.2921646746347942</v>
+      </c>
+      <c r="G2">
+        <v>0.2632575757575757</v>
+      </c>
+      <c r="H2">
+        <v>0.2534653465346535</v>
+      </c>
+      <c r="I2">
+        <v>0.2921646746347942</v>
+      </c>
+      <c r="J2">
+        <v>0.2632575757575757</v>
+      </c>
+      <c r="K2">
+        <v>0.2806451612903226</v>
+      </c>
+      <c r="L2">
+        <v>0.2921646746347942</v>
+      </c>
+      <c r="M2">
+        <v>0.2805555555555556</v>
+      </c>
+      <c r="N2">
+        <v>0.2404092071611253</v>
+      </c>
+      <c r="O2">
+        <v>0.2921646746347942</v>
+      </c>
+      <c r="P2">
+        <v>0.2805555555555556</v>
+      </c>
+      <c r="Q2">
+        <v>0.2724137931034483</v>
+      </c>
+      <c r="R2">
+        <v>0.3817204301075269</v>
+      </c>
+      <c r="S2">
+        <v>0.361800346220427</v>
+      </c>
+      <c r="T2">
+        <v>0.3455637091394263</v>
+      </c>
+      <c r="U2">
+        <v>0.3817204301075269</v>
+      </c>
+      <c r="V2">
+        <v>0.361800346220427</v>
+      </c>
+      <c r="W2">
+        <v>0.3513011152416357</v>
+      </c>
+      <c r="X2">
+        <v>0.7154178674351584</v>
+      </c>
+      <c r="Y2">
+        <v>0.7984361424847958</v>
+      </c>
+      <c r="Z2">
+        <v>0.3817204301075269</v>
+      </c>
+      <c r="AA2">
+        <v>0.361800346220427</v>
+      </c>
+      <c r="AB2">
+        <v>0.3586367157242448</v>
+      </c>
+      <c r="AC2">
+        <v>0.7154178674351584</v>
+      </c>
+      <c r="AD2">
+        <v>0.800952380952381</v>
+      </c>
+      <c r="AE2">
+        <v>0.3817204301075269</v>
+      </c>
+      <c r="AF2">
+        <v>0.361800346220427</v>
+      </c>
+      <c r="AG2">
+        <v>0.3605324074074074</v>
+      </c>
+      <c r="AH2">
+        <v>0.3817204301075269</v>
+      </c>
+      <c r="AI2">
+        <v>0.3626716604244694</v>
+      </c>
+      <c r="AJ2">
+        <v>0.360479797979798</v>
+      </c>
+      <c r="AK2">
+        <v>0.7154178674351584</v>
+      </c>
+      <c r="AL2">
+        <v>0.7549103330486764</v>
+      </c>
+      <c r="AM2">
+        <v>0.3817204301075269</v>
+      </c>
+      <c r="AN2">
+        <v>0.361800346220427</v>
+      </c>
+      <c r="AO2">
+        <v>0.3521524347212421</v>
+      </c>
+      <c r="AP2">
+        <v>0.7154178674351584</v>
+      </c>
+      <c r="AQ2">
+        <v>0.3817204301075269</v>
+      </c>
+      <c r="AR2">
+        <v>0.361800346220427</v>
+      </c>
+      <c r="AS2">
+        <v>0.7154178674351584</v>
+      </c>
+      <c r="AT2">
+        <v>0.7346153846153847</v>
+      </c>
+      <c r="AU2">
+        <v>0.3817204301075269</v>
+      </c>
+      <c r="AV2">
+        <v>0.3626716604244694</v>
+      </c>
+      <c r="AW2">
+        <v>0.3589093214965124</v>
+      </c>
+      <c r="AX2">
+        <v>0.7154178674351584</v>
+      </c>
+      <c r="AY2">
+        <v>0.7360126083530338</v>
+      </c>
+      <c r="AZ2">
+        <v>0.4787657597876576</v>
+      </c>
+      <c r="BA2">
+        <v>0.4510948905109489</v>
+      </c>
+      <c r="BB2">
+        <v>0.7154178674351584</v>
+      </c>
+      <c r="BC2">
+        <v>0.710955710955711</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55">
+      <c r="A3" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B3">
+        <v>3522</v>
+      </c>
+      <c r="C3">
+        <v>0.5019875070982396</v>
+      </c>
+      <c r="D3">
+        <v>0.008426234876814374</v>
+      </c>
+      <c r="E3">
+        <v>176.1</v>
+      </c>
+      <c r="F3">
+        <v>0.2480376766091052</v>
+      </c>
+      <c r="G3">
+        <v>0.2310924369747899</v>
+      </c>
+      <c r="H3">
+        <v>0.2195652173913044</v>
+      </c>
+      <c r="I3">
+        <v>0.2480376766091052</v>
+      </c>
+      <c r="J3">
+        <v>0.2310924369747899</v>
+      </c>
+      <c r="K3">
+        <v>0.2024291497975708</v>
+      </c>
+      <c r="L3">
+        <v>0.2480376766091052</v>
+      </c>
+      <c r="M3">
+        <v>0.2361563517915309</v>
+      </c>
+      <c r="N3">
+        <v>0.212962962962963</v>
+      </c>
+      <c r="O3">
+        <v>0.2480376766091052</v>
+      </c>
+      <c r="P3">
+        <v>0.2361563517915309</v>
+      </c>
+      <c r="Q3">
+        <v>0.208695652173913</v>
+      </c>
+      <c r="R3">
+        <v>0.3089214380825566</v>
+      </c>
+      <c r="S3">
+        <v>0.2896995708154507</v>
+      </c>
+      <c r="T3">
+        <v>0.2837729816147082</v>
+      </c>
+      <c r="U3">
+        <v>0.3089214380825566</v>
+      </c>
+      <c r="V3">
+        <v>0.2896995708154507</v>
+      </c>
+      <c r="W3">
+        <v>0.2887060583395662</v>
+      </c>
+      <c r="X3">
+        <v>0.7204116638078902</v>
+      </c>
+      <c r="Y3">
+        <v>0.8132780082987552</v>
+      </c>
+      <c r="Z3">
+        <v>0.3089214380825566</v>
+      </c>
+      <c r="AA3">
+        <v>0.2896995708154507</v>
+      </c>
+      <c r="AB3">
+        <v>0.2744186046511628</v>
+      </c>
+      <c r="AC3">
+        <v>0.7204116638078902</v>
+      </c>
+      <c r="AD3">
+        <v>0.8162583518930958</v>
+      </c>
+      <c r="AE3">
+        <v>0.3089214380825566</v>
+      </c>
+      <c r="AF3">
+        <v>0.2896995708154507</v>
+      </c>
+      <c r="AG3">
+        <v>0.2914244186046512</v>
+      </c>
+      <c r="AH3">
+        <v>0.3089214380825566</v>
+      </c>
+      <c r="AI3">
+        <v>0.3014925373134328</v>
+      </c>
+      <c r="AJ3">
+        <v>0.299324831207802</v>
+      </c>
+      <c r="AK3">
+        <v>0.7204116638078902</v>
+      </c>
+      <c r="AL3">
+        <v>0.7753479125248509</v>
+      </c>
+      <c r="AM3">
+        <v>0.3089214380825566</v>
+      </c>
+      <c r="AN3">
+        <v>0.2896995708154507</v>
+      </c>
+      <c r="AO3">
+        <v>0.2675276752767528</v>
+      </c>
+      <c r="AP3">
+        <v>0.7204116638078902</v>
+      </c>
+      <c r="AQ3">
+        <v>0.3089214380825566</v>
+      </c>
+      <c r="AR3">
+        <v>0.2896995708154507</v>
+      </c>
+      <c r="AS3">
+        <v>0.7204116638078902</v>
+      </c>
+      <c r="AT3">
+        <v>0.7448979591836735</v>
+      </c>
+      <c r="AU3">
+        <v>0.3089214380825566</v>
+      </c>
+      <c r="AV3">
+        <v>0.3014925373134328</v>
+      </c>
+      <c r="AW3">
+        <v>0.2995495495495495</v>
+      </c>
+      <c r="AX3">
+        <v>0.7204116638078902</v>
+      </c>
+      <c r="AY3">
+        <v>0.7571569595261599</v>
+      </c>
+      <c r="AZ3">
+        <v>0.3938879456706282</v>
+      </c>
+      <c r="BA3">
+        <v>0.3635509628933772</v>
+      </c>
+      <c r="BB3">
+        <v>0.7204116638078902</v>
+      </c>
+      <c r="BC3">
+        <v>0.7172727272727273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:55">
+      <c r="A4" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B4">
+        <v>4232</v>
+      </c>
+      <c r="C4">
+        <v>0.4468336483931947</v>
+      </c>
+      <c r="D4">
+        <v>0.007643271727985883</v>
+      </c>
+      <c r="E4">
+        <v>211.6</v>
+      </c>
+      <c r="F4">
+        <v>0.1554828150572831</v>
+      </c>
+      <c r="G4">
+        <v>0.1411483253588517</v>
+      </c>
+      <c r="H4">
+        <v>0.1306532663316583</v>
+      </c>
+      <c r="I4">
+        <v>0.1554828150572831</v>
+      </c>
+      <c r="J4">
+        <v>0.1411483253588517</v>
+      </c>
+      <c r="K4">
+        <v>0.148936170212766</v>
+      </c>
+      <c r="L4">
+        <v>0.1554828150572831</v>
+      </c>
+      <c r="M4">
+        <v>0.1393728222996516</v>
+      </c>
+      <c r="N4">
+        <v>0.11</v>
+      </c>
+      <c r="O4">
+        <v>0.1554828150572831</v>
+      </c>
+      <c r="P4">
+        <v>0.1393728222996516</v>
+      </c>
+      <c r="Q4">
+        <v>0.1371681415929203</v>
+      </c>
+      <c r="R4">
+        <v>0.2216343327454439</v>
+      </c>
+      <c r="S4">
+        <v>0.20125</v>
+      </c>
+      <c r="T4">
+        <v>0.1906474820143885</v>
+      </c>
+      <c r="U4">
+        <v>0.2216343327454439</v>
+      </c>
+      <c r="V4">
+        <v>0.20125</v>
+      </c>
+      <c r="W4">
+        <v>0.1944818304172275</v>
+      </c>
+      <c r="X4">
+        <v>0.6975609756097561</v>
+      </c>
+      <c r="Y4">
+        <v>0.7483870967741936</v>
+      </c>
+      <c r="Z4">
+        <v>0.2216343327454439</v>
+      </c>
+      <c r="AA4">
+        <v>0.20125</v>
+      </c>
+      <c r="AB4">
+        <v>0.196031746031746</v>
+      </c>
+      <c r="AC4">
+        <v>0.6975609756097561</v>
+      </c>
+      <c r="AD4">
+        <v>0.7489139878366637</v>
+      </c>
+      <c r="AE4">
+        <v>0.2216343327454439</v>
+      </c>
+      <c r="AF4">
+        <v>0.20125</v>
+      </c>
+      <c r="AG4">
+        <v>0.2020138451856514</v>
+      </c>
+      <c r="AH4">
+        <v>0.2216343327454439</v>
+      </c>
+      <c r="AI4">
+        <v>0.2080217539089055</v>
+      </c>
+      <c r="AJ4">
+        <v>0.2081911262798635</v>
+      </c>
+      <c r="AK4">
+        <v>0.6975609756097561</v>
+      </c>
+      <c r="AL4">
+        <v>0.7364470391993327</v>
+      </c>
+      <c r="AM4">
+        <v>0.2216343327454439</v>
+      </c>
+      <c r="AN4">
+        <v>0.20125</v>
+      </c>
+      <c r="AO4">
+        <v>0.1907514450867052</v>
+      </c>
+      <c r="AP4">
+        <v>0.6975609756097561</v>
+      </c>
+      <c r="AQ4">
+        <v>0.2216343327454439</v>
+      </c>
+      <c r="AR4">
+        <v>0.20125</v>
+      </c>
+      <c r="AS4">
+        <v>0.6975609756097561</v>
+      </c>
+      <c r="AT4">
+        <v>0.7037582903463523</v>
+      </c>
+      <c r="AU4">
+        <v>0.2216343327454439</v>
+      </c>
+      <c r="AV4">
+        <v>0.2080217539089055</v>
+      </c>
+      <c r="AW4">
+        <v>0.2077922077922078</v>
+      </c>
+      <c r="AX4">
+        <v>0.6975609756097561</v>
+      </c>
+      <c r="AY4">
+        <v>0.7044072948328267</v>
+      </c>
+      <c r="AZ4">
+        <v>0.3181980693600286</v>
+      </c>
+      <c r="BA4">
+        <v>0.2906116088819634</v>
+      </c>
+      <c r="BB4">
+        <v>0.6975609756097561</v>
+      </c>
+      <c r="BC4">
+        <v>0.6946508172362555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55">
+      <c r="A5" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B5">
+        <v>3560</v>
+      </c>
+      <c r="C5">
+        <v>0.377808988764045</v>
+      </c>
+      <c r="D5">
+        <v>0.008127070281522939</v>
+      </c>
+      <c r="E5">
+        <v>178</v>
+      </c>
+      <c r="F5">
+        <v>0.1053484602917342</v>
+      </c>
+      <c r="G5">
+        <v>0.08669354838709678</v>
+      </c>
+      <c r="H5">
+        <v>0.0778688524590164</v>
+      </c>
+      <c r="I5">
+        <v>0.1053484602917342</v>
+      </c>
+      <c r="J5">
+        <v>0.08669354838709678</v>
+      </c>
+      <c r="K5">
+        <v>0.09642857142857143</v>
+      </c>
+      <c r="L5">
+        <v>0.1053484602917342</v>
+      </c>
+      <c r="M5">
+        <v>0.09437086092715231</v>
+      </c>
+      <c r="N5">
+        <v>0.07255520504731862</v>
+      </c>
+      <c r="O5">
+        <v>0.1053484602917342</v>
+      </c>
+      <c r="P5">
+        <v>0.09437086092715231</v>
+      </c>
+      <c r="Q5">
+        <v>0.06389776357827476</v>
+      </c>
+      <c r="R5">
+        <v>0.1603206412825651</v>
+      </c>
+      <c r="S5">
+        <v>0.1433591004919185</v>
+      </c>
+      <c r="T5">
+        <v>0.133384734001542</v>
+      </c>
+      <c r="U5">
+        <v>0.1603206412825651</v>
+      </c>
+      <c r="V5">
+        <v>0.1433591004919185</v>
+      </c>
+      <c r="W5">
+        <v>0.1386430678466077</v>
+      </c>
+      <c r="X5">
+        <v>0.638228055783429</v>
+      </c>
+      <c r="Y5">
+        <v>0.6972034715525555</v>
+      </c>
+      <c r="Z5">
+        <v>0.1603206412825651</v>
+      </c>
+      <c r="AA5">
+        <v>0.1433591004919185</v>
+      </c>
+      <c r="AB5">
+        <v>0.1363265306122449</v>
+      </c>
+      <c r="AC5">
+        <v>0.638228055783429</v>
+      </c>
+      <c r="AD5">
+        <v>0.6984771573604061</v>
+      </c>
+      <c r="AE5">
+        <v>0.1603206412825651</v>
+      </c>
+      <c r="AF5">
+        <v>0.1433591004919185</v>
+      </c>
+      <c r="AG5">
+        <v>0.144793152639087</v>
+      </c>
+      <c r="AH5">
+        <v>0.1603206412825651</v>
+      </c>
+      <c r="AI5">
+        <v>0.1482300884955752</v>
+      </c>
+      <c r="AJ5">
+        <v>0.1477104874446086</v>
+      </c>
+      <c r="AK5">
+        <v>0.638228055783429</v>
+      </c>
+      <c r="AL5">
+        <v>0.6827852998065764</v>
+      </c>
+      <c r="AM5">
+        <v>0.1603206412825651</v>
+      </c>
+      <c r="AN5">
+        <v>0.1433591004919185</v>
+      </c>
+      <c r="AO5">
+        <v>0.1376481312670921</v>
+      </c>
+      <c r="AP5">
+        <v>0.638228055783429</v>
+      </c>
+      <c r="AQ5">
+        <v>0.1603206412825651</v>
+      </c>
+      <c r="AR5">
+        <v>0.1433591004919185</v>
+      </c>
+      <c r="AS5">
+        <v>0.638228055783429</v>
+      </c>
+      <c r="AT5">
+        <v>0.6506968641114983</v>
+      </c>
+      <c r="AU5">
+        <v>0.1603206412825651</v>
+      </c>
+      <c r="AV5">
+        <v>0.1482300884955752</v>
+      </c>
+      <c r="AW5">
+        <v>0.147819660014782</v>
+      </c>
+      <c r="AX5">
+        <v>0.638228055783429</v>
+      </c>
+      <c r="AY5">
+        <v>0.6575091575091575</v>
+      </c>
+      <c r="AZ5">
+        <v>0.2422041862451944</v>
+      </c>
+      <c r="BA5">
+        <v>0.2161290322580645</v>
+      </c>
+      <c r="BB5">
+        <v>0.638228055783429</v>
+      </c>
+      <c r="BC5">
+        <v>0.636675235646958</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55">
+      <c r="A6" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B6">
+        <v>4375</v>
+      </c>
+      <c r="C6">
+        <v>0.3494857142857143</v>
+      </c>
+      <c r="D6">
+        <v>0.007209476721260907</v>
+      </c>
+      <c r="E6">
+        <v>218.75</v>
+      </c>
+      <c r="F6">
+        <v>0.08011049723756906</v>
+      </c>
+      <c r="G6">
+        <v>0.07524752475247524</v>
+      </c>
+      <c r="H6">
+        <v>0.07489878542510121</v>
+      </c>
+      <c r="I6">
+        <v>0.08011049723756906</v>
+      </c>
+      <c r="J6">
+        <v>0.07524752475247524</v>
+      </c>
+      <c r="K6">
+        <v>0.06853582554517133</v>
+      </c>
+      <c r="L6">
+        <v>0.08011049723756906</v>
+      </c>
+      <c r="M6">
+        <v>0.07845934379457917</v>
+      </c>
+      <c r="N6">
+        <v>0.06417112299465241</v>
+      </c>
+      <c r="O6">
+        <v>0.08011049723756906</v>
+      </c>
+      <c r="P6">
+        <v>0.07845934379457917</v>
+      </c>
+      <c r="Q6">
+        <v>0.04984423676012461</v>
+      </c>
+      <c r="R6">
+        <v>0.1420794774088187</v>
+      </c>
+      <c r="S6">
+        <v>0.1314580941446613</v>
+      </c>
+      <c r="T6">
+        <v>0.1213333333333333</v>
+      </c>
+      <c r="U6">
+        <v>0.1420794774088187</v>
+      </c>
+      <c r="V6">
+        <v>0.1314580941446613</v>
+      </c>
+      <c r="W6">
+        <v>0.1280148423005566</v>
+      </c>
+      <c r="X6">
+        <v>0.6369426751592356</v>
+      </c>
+      <c r="Y6">
+        <v>0.6826051112943117</v>
+      </c>
+      <c r="Z6">
+        <v>0.1420794774088187</v>
+      </c>
+      <c r="AA6">
+        <v>0.1314580941446613</v>
+      </c>
+      <c r="AB6">
+        <v>0.1312217194570136</v>
+      </c>
+      <c r="AC6">
+        <v>0.6369426751592356</v>
+      </c>
+      <c r="AD6">
+        <v>0.6885688568856886</v>
+      </c>
+      <c r="AE6">
+        <v>0.1420794774088187</v>
+      </c>
+      <c r="AF6">
+        <v>0.1314580941446613</v>
+      </c>
+      <c r="AG6">
+        <v>0.1310507674144038</v>
+      </c>
+      <c r="AH6">
+        <v>0.1420794774088187</v>
+      </c>
+      <c r="AI6">
+        <v>0.1292170591979631</v>
+      </c>
+      <c r="AJ6">
+        <v>0.1289087428206765</v>
+      </c>
+      <c r="AK6">
+        <v>0.6369426751592356</v>
+      </c>
+      <c r="AL6">
+        <v>0.6565377532228361</v>
+      </c>
+      <c r="AM6">
+        <v>0.1420794774088187</v>
+      </c>
+      <c r="AN6">
+        <v>0.1314580941446613</v>
+      </c>
+      <c r="AO6">
+        <v>0.1292824822236587</v>
+      </c>
+      <c r="AP6">
+        <v>0.6369426751592356</v>
+      </c>
+      <c r="AQ6">
+        <v>0.1420794774088187</v>
+      </c>
+      <c r="AR6">
+        <v>0.1314580941446613</v>
+      </c>
+      <c r="AS6">
+        <v>0.6369426751592356</v>
+      </c>
+      <c r="AT6">
+        <v>0.6434456928838951</v>
+      </c>
+      <c r="AU6">
+        <v>0.1420794774088187</v>
+      </c>
+      <c r="AV6">
+        <v>0.1292170591979631</v>
+      </c>
+      <c r="AW6">
+        <v>0.129156010230179</v>
+      </c>
+      <c r="AX6">
+        <v>0.6369426751592356</v>
+      </c>
+      <c r="AY6">
+        <v>0.6481774960380349</v>
+      </c>
+      <c r="AZ6">
+        <v>0.212356515867657</v>
+      </c>
+      <c r="BA6">
+        <v>0.1887477313974592</v>
+      </c>
+      <c r="BB6">
+        <v>0.6369426751592356</v>
+      </c>
+      <c r="BC6">
+        <v>0.6384439359267735</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55">
+      <c r="A7" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B7">
+        <v>3341</v>
+      </c>
+      <c r="C7">
+        <v>0.2648907512720742</v>
+      </c>
+      <c r="D7">
+        <v>0.007635475844113779</v>
+      </c>
+      <c r="E7">
+        <v>167.05</v>
+      </c>
+      <c r="F7">
+        <v>0.03839732888146911</v>
+      </c>
+      <c r="G7">
+        <v>0.03023255813953488</v>
+      </c>
+      <c r="H7">
+        <v>0.02857142857142857</v>
+      </c>
+      <c r="I7">
+        <v>0.03839732888146911</v>
+      </c>
+      <c r="J7">
+        <v>0.03023255813953488</v>
+      </c>
+      <c r="K7">
+        <v>0.01915708812260536</v>
+      </c>
+      <c r="L7">
+        <v>0.03839732888146911</v>
+      </c>
+      <c r="M7">
+        <v>0.03747870528109029</v>
+      </c>
+      <c r="N7">
+        <v>0.02160493827160494</v>
+      </c>
+      <c r="O7">
+        <v>0.03839732888146911</v>
+      </c>
+      <c r="P7">
+        <v>0.03747870528109029</v>
+      </c>
+      <c r="Q7">
+        <v>0.0316622691292876</v>
+      </c>
+      <c r="R7">
+        <v>0.07313540912382331</v>
+      </c>
+      <c r="S7">
+        <v>0.06566037735849056</v>
+      </c>
+      <c r="T7">
+        <v>0.05263157894736842</v>
+      </c>
+      <c r="U7">
+        <v>0.07313540912382331</v>
+      </c>
+      <c r="V7">
+        <v>0.06566037735849056</v>
+      </c>
+      <c r="W7">
+        <v>0.05709624796084829</v>
+      </c>
+      <c r="X7">
+        <v>0.5306691449814126</v>
+      </c>
+      <c r="Y7">
+        <v>0.5651697699890471</v>
+      </c>
+      <c r="Z7">
+        <v>0.07313540912382331</v>
+      </c>
+      <c r="AA7">
+        <v>0.06566037735849056</v>
+      </c>
+      <c r="AB7">
+        <v>0.05421103581800581</v>
+      </c>
+      <c r="AC7">
+        <v>0.5306691449814126</v>
+      </c>
+      <c r="AD7">
+        <v>0.5649122807017544</v>
+      </c>
+      <c r="AE7">
+        <v>0.07313540912382331</v>
+      </c>
+      <c r="AF7">
+        <v>0.06566037735849056</v>
+      </c>
+      <c r="AG7">
+        <v>0.06528417818740399</v>
+      </c>
+      <c r="AH7">
+        <v>0.07313540912382331</v>
+      </c>
+      <c r="AI7">
+        <v>0.05756013745704467</v>
+      </c>
+      <c r="AJ7">
+        <v>0.05598621877691645</v>
+      </c>
+      <c r="AK7">
+        <v>0.5306691449814126</v>
+      </c>
+      <c r="AL7">
+        <v>0.5506257110352674</v>
+      </c>
+      <c r="AM7">
+        <v>0.07313540912382331</v>
+      </c>
+      <c r="AN7">
+        <v>0.06566037735849056</v>
+      </c>
+      <c r="AO7">
+        <v>0.06143344709897611</v>
+      </c>
+      <c r="AP7">
+        <v>0.5306691449814126</v>
+      </c>
+      <c r="AQ7">
+        <v>0.07313540912382331</v>
+      </c>
+      <c r="AR7">
+        <v>0.06566037735849056</v>
+      </c>
+      <c r="AS7">
+        <v>0.5306691449814126</v>
+      </c>
+      <c r="AT7">
+        <v>0.5401234567901234</v>
+      </c>
+      <c r="AU7">
+        <v>0.07313540912382331</v>
+      </c>
+      <c r="AV7">
+        <v>0.05756013745704467</v>
+      </c>
+      <c r="AW7">
+        <v>0.05613126079447323</v>
+      </c>
+      <c r="AX7">
+        <v>0.5306691449814126</v>
+      </c>
+      <c r="AY7">
+        <v>0.537180910099889</v>
+      </c>
+      <c r="AZ7">
+        <v>0.1386313465783665</v>
+      </c>
+      <c r="BA7">
+        <v>0.1164772727272727</v>
+      </c>
+      <c r="BB7">
+        <v>0.5306691449814126</v>
+      </c>
+      <c r="BC7">
+        <v>0.5284872298624754</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55">
+      <c r="A8" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B8">
+        <v>4322</v>
+      </c>
+      <c r="C8">
+        <v>0.2320684868116613</v>
+      </c>
+      <c r="D8">
+        <v>0.006422101970115271</v>
+      </c>
+      <c r="E8">
+        <v>216.1</v>
+      </c>
+      <c r="F8">
+        <v>0.0467065868263473</v>
+      </c>
+      <c r="G8">
+        <v>0.03565640194489465</v>
+      </c>
+      <c r="H8">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="I8">
+        <v>0.0467065868263473</v>
+      </c>
+      <c r="J8">
+        <v>0.03565640194489465</v>
+      </c>
+      <c r="K8">
+        <v>0.0325</v>
+      </c>
+      <c r="L8">
+        <v>0.0467065868263473</v>
+      </c>
+      <c r="M8">
+        <v>0.03593556381660471</v>
+      </c>
+      <c r="N8">
+        <v>0.01590909090909091</v>
+      </c>
+      <c r="O8">
+        <v>0.0467065868263473</v>
+      </c>
+      <c r="P8">
+        <v>0.03593556381660471</v>
+      </c>
+      <c r="Q8">
+        <v>0.02133333333333333</v>
+      </c>
+      <c r="R8">
+        <v>0.07336523125996811</v>
+      </c>
+      <c r="S8">
+        <v>0.06030150753768844</v>
+      </c>
+      <c r="T8">
+        <v>0.05276381909547739</v>
+      </c>
+      <c r="U8">
+        <v>0.07336523125996811</v>
+      </c>
+      <c r="V8">
+        <v>0.06030150753768844</v>
+      </c>
+      <c r="W8">
+        <v>0.05562060889929742</v>
+      </c>
+      <c r="X8">
+        <v>0.4705014749262537</v>
+      </c>
+      <c r="Y8">
+        <v>0.5190972222222222</v>
+      </c>
+      <c r="Z8">
+        <v>0.07336523125996811</v>
+      </c>
+      <c r="AA8">
+        <v>0.06030150753768844</v>
+      </c>
+      <c r="AB8">
+        <v>0.05145565335138795</v>
+      </c>
+      <c r="AC8">
+        <v>0.4705014749262537</v>
+      </c>
+      <c r="AD8">
+        <v>0.5285977859778598</v>
+      </c>
+      <c r="AE8">
+        <v>0.07336523125996811</v>
+      </c>
+      <c r="AF8">
+        <v>0.06030150753768844</v>
+      </c>
+      <c r="AG8">
+        <v>0.05938375350140056</v>
+      </c>
+      <c r="AH8">
+        <v>0.07336523125996811</v>
+      </c>
+      <c r="AI8">
+        <v>0.06430288461538461</v>
+      </c>
+      <c r="AJ8">
+        <v>0.06332931242460796</v>
+      </c>
+      <c r="AK8">
+        <v>0.4705014749262537</v>
+      </c>
+      <c r="AL8">
+        <v>0.5138023152270703</v>
+      </c>
+      <c r="AM8">
+        <v>0.07336523125996811</v>
+      </c>
+      <c r="AN8">
+        <v>0.06030150753768844</v>
+      </c>
+      <c r="AO8">
+        <v>0.05520304568527919</v>
+      </c>
+      <c r="AP8">
+        <v>0.4705014749262537</v>
+      </c>
+      <c r="AQ8">
+        <v>0.07336523125996811</v>
+      </c>
+      <c r="AR8">
+        <v>0.06030150753768844</v>
+      </c>
+      <c r="AS8">
+        <v>0.4705014749262537</v>
+      </c>
+      <c r="AT8">
+        <v>0.4748822605965463</v>
+      </c>
+      <c r="AU8">
+        <v>0.07336523125996811</v>
+      </c>
+      <c r="AV8">
+        <v>0.06430288461538461</v>
+      </c>
+      <c r="AW8">
+        <v>0.06238643246517262</v>
+      </c>
+      <c r="AX8">
+        <v>0.4705014749262537</v>
+      </c>
+      <c r="AY8">
+        <v>0.4773289365210223</v>
+      </c>
+      <c r="AZ8">
+        <v>0.1230613621038436</v>
+      </c>
+      <c r="BA8">
+        <v>0.1062455132806892</v>
+      </c>
+      <c r="BB8">
+        <v>0.4705014749262537</v>
+      </c>
+      <c r="BC8">
+        <v>0.4759316770186335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55">
+      <c r="A9" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>4145</v>
+      </c>
+      <c r="C9">
+        <v>0.2130277442702051</v>
+      </c>
+      <c r="D9">
+        <v>0.006360451156136092</v>
+      </c>
+      <c r="E9">
+        <v>207.25</v>
+      </c>
+      <c r="F9">
+        <v>0.03243847874720358</v>
+      </c>
+      <c r="G9">
+        <v>0.0202808112324493</v>
+      </c>
+      <c r="H9">
+        <v>0.01628664495114007</v>
+      </c>
+      <c r="I9">
+        <v>0.03243847874720358</v>
+      </c>
+      <c r="J9">
+        <v>0.0202808112324493</v>
+      </c>
+      <c r="K9">
+        <v>0.0131578947368421</v>
+      </c>
+      <c r="L9">
+        <v>0.03243847874720358</v>
+      </c>
+      <c r="M9">
+        <v>0.02686915887850467</v>
+      </c>
+      <c r="N9">
+        <v>0.02040816326530612</v>
+      </c>
+      <c r="O9">
+        <v>0.03243847874720358</v>
+      </c>
+      <c r="P9">
+        <v>0.02686915887850467</v>
+      </c>
+      <c r="Q9">
+        <v>0.01470588235294118</v>
+      </c>
+      <c r="R9">
+        <v>0.0655226209048362</v>
+      </c>
+      <c r="S9">
+        <v>0.05774569683509161</v>
+      </c>
+      <c r="T9">
+        <v>0.05212968849332485</v>
+      </c>
+      <c r="U9">
+        <v>0.0655226209048362</v>
+      </c>
+      <c r="V9">
+        <v>0.05774569683509161</v>
+      </c>
+      <c r="W9">
+        <v>0.05322294500295683</v>
+      </c>
+      <c r="X9">
+        <v>0.4353954581049335</v>
+      </c>
+      <c r="Y9">
+        <v>0.4878993223620523</v>
+      </c>
+      <c r="Z9">
+        <v>0.0655226209048362</v>
+      </c>
+      <c r="AA9">
+        <v>0.05774569683509161</v>
+      </c>
+      <c r="AB9">
+        <v>0.0499001996007984</v>
+      </c>
+      <c r="AC9">
+        <v>0.4353954581049335</v>
+      </c>
+      <c r="AD9">
+        <v>0.4948559670781893</v>
+      </c>
+      <c r="AE9">
+        <v>0.0655226209048362</v>
+      </c>
+      <c r="AF9">
+        <v>0.05774569683509161</v>
+      </c>
+      <c r="AG9">
+        <v>0.05752961082910321</v>
+      </c>
+      <c r="AH9">
+        <v>0.0655226209048362</v>
+      </c>
+      <c r="AI9">
+        <v>0.05765765765765766</v>
+      </c>
+      <c r="AJ9">
+        <v>0.05693519079345851</v>
+      </c>
+      <c r="AK9">
+        <v>0.4353954581049335</v>
+      </c>
+      <c r="AL9">
+        <v>0.4768339768339768</v>
+      </c>
+      <c r="AM9">
+        <v>0.0655226209048362</v>
+      </c>
+      <c r="AN9">
+        <v>0.05774569683509161</v>
+      </c>
+      <c r="AO9">
+        <v>0.05800604229607251</v>
+      </c>
+      <c r="AP9">
+        <v>0.4353954581049335</v>
+      </c>
+      <c r="AQ9">
+        <v>0.0655226209048362</v>
+      </c>
+      <c r="AR9">
+        <v>0.05774569683509161</v>
+      </c>
+      <c r="AS9">
+        <v>0.4353954581049335</v>
+      </c>
+      <c r="AT9">
+        <v>0.4428807947019868</v>
+      </c>
+      <c r="AU9">
+        <v>0.0655226209048362</v>
+      </c>
+      <c r="AV9">
+        <v>0.05765765765765766</v>
+      </c>
+      <c r="AW9">
+        <v>0.05643203883495146</v>
+      </c>
+      <c r="AX9">
+        <v>0.4353954581049335</v>
+      </c>
+      <c r="AY9">
+        <v>0.4508414526129318</v>
+      </c>
+      <c r="AZ9">
+        <v>0.1140167364016736</v>
+      </c>
+      <c r="BA9">
+        <v>0.09418070444104135</v>
+      </c>
+      <c r="BB9">
+        <v>0.4353954581049335</v>
+      </c>
+      <c r="BC9">
+        <v>0.4383223684210527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55">
+      <c r="A10" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B10">
+        <v>3486</v>
+      </c>
+      <c r="C10">
+        <v>0.2240390131956397</v>
+      </c>
+      <c r="D10">
+        <v>0.007062856420827443</v>
+      </c>
+      <c r="E10">
+        <v>174.3</v>
+      </c>
+      <c r="F10">
+        <v>0.05236270753512133</v>
+      </c>
+      <c r="G10">
+        <v>0.04528985507246377</v>
+      </c>
+      <c r="H10">
+        <v>0.03802281368821293</v>
+      </c>
+      <c r="I10">
+        <v>0.05236270753512133</v>
+      </c>
+      <c r="J10">
+        <v>0.04528985507246377</v>
+      </c>
+      <c r="K10">
+        <v>0.0325</v>
+      </c>
+      <c r="L10">
+        <v>0.05236270753512133</v>
+      </c>
+      <c r="M10">
+        <v>0.04582210242587601</v>
+      </c>
+      <c r="N10">
+        <v>0.03551912568306011</v>
+      </c>
+      <c r="O10">
+        <v>0.05236270753512133</v>
+      </c>
+      <c r="P10">
+        <v>0.04582210242587601</v>
+      </c>
+      <c r="Q10">
+        <v>0.03865979381443299</v>
+      </c>
+      <c r="R10">
+        <v>0.0762660158633313</v>
+      </c>
+      <c r="S10">
+        <v>0.06723237597911227</v>
+      </c>
+      <c r="T10">
+        <v>0.06113207547169811</v>
+      </c>
+      <c r="U10">
+        <v>0.0762660158633313</v>
+      </c>
+      <c r="V10">
+        <v>0.06723237597911227</v>
+      </c>
+      <c r="W10">
+        <v>0.06388888888888888</v>
+      </c>
+      <c r="X10">
+        <v>0.4488107549120993</v>
+      </c>
+      <c r="Y10">
+        <v>0.5050890585241731</v>
+      </c>
+      <c r="Z10">
+        <v>0.0762660158633313</v>
+      </c>
+      <c r="AA10">
+        <v>0.06723237597911227</v>
+      </c>
+      <c r="AB10">
+        <v>0.06354249404289118</v>
+      </c>
+      <c r="AC10">
+        <v>0.4488107549120993</v>
+      </c>
+      <c r="AD10">
+        <v>0.5213793103448275</v>
+      </c>
+      <c r="AE10">
+        <v>0.0762660158633313</v>
+      </c>
+      <c r="AF10">
+        <v>0.06723237597911227</v>
+      </c>
+      <c r="AG10">
+        <v>0.06737120211360634</v>
+      </c>
+      <c r="AH10">
+        <v>0.0762660158633313</v>
+      </c>
+      <c r="AI10">
+        <v>0.06874557051736357</v>
+      </c>
+      <c r="AJ10">
+        <v>0.06743185078909612</v>
+      </c>
+      <c r="AK10">
+        <v>0.4488107549120993</v>
+      </c>
+      <c r="AL10">
+        <v>0.4889466840052016</v>
+      </c>
+      <c r="AM10">
+        <v>0.0762660158633313</v>
+      </c>
+      <c r="AN10">
+        <v>0.06723237597911227</v>
+      </c>
+      <c r="AO10">
+        <v>0.06423982869379015</v>
+      </c>
+      <c r="AP10">
+        <v>0.4488107549120993</v>
+      </c>
+      <c r="AQ10">
+        <v>0.0762660158633313</v>
+      </c>
+      <c r="AR10">
+        <v>0.06723237597911227</v>
+      </c>
+      <c r="AS10">
+        <v>0.4488107549120993</v>
+      </c>
+      <c r="AT10">
+        <v>0.4539400665926748</v>
+      </c>
+      <c r="AU10">
+        <v>0.0762660158633313</v>
+      </c>
+      <c r="AV10">
+        <v>0.06874557051736357</v>
+      </c>
+      <c r="AW10">
+        <v>0.06647398843930635</v>
+      </c>
+      <c r="AX10">
+        <v>0.4488107549120993</v>
+      </c>
+      <c r="AY10">
+        <v>0.4652532391048292</v>
+      </c>
+      <c r="AZ10">
+        <v>0.1377530766177054</v>
+      </c>
+      <c r="BA10">
+        <v>0.1181619256017506</v>
+      </c>
+      <c r="BB10">
+        <v>0.4488107549120993</v>
+      </c>
+      <c r="BC10">
+        <v>0.4580573951434879</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>